<commit_message>
New example files updated.
</commit_message>
<xml_diff>
--- a/example/e2fsprogs-1.39/input/e2fsprogs-1.39-INV.xlsx
+++ b/example/e2fsprogs-1.39/input/e2fsprogs-1.39-INV.xlsx
@@ -361,9 +361,6 @@
     <t>Copyright (c) 1997-2004 Theodore Ts'o</t>
   </si>
   <si>
-    <t>dje_license</t>
-  </si>
-  <si>
     <t>notice_file</t>
   </si>
   <si>
@@ -518,6 +515,9 @@
   </si>
   <si>
     <t>UlrichWindl.LICENSE</t>
+  </si>
+  <si>
+    <t>dje_license_key</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1203,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>69</v>
@@ -1218,19 +1218,19 @@
         <v>105</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>108</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>8</v>
@@ -1253,7 +1253,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>72</v>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>107</v>
@@ -1284,10 +1284,10 @@
     </row>
     <row r="3" spans="1:16" s="3" customFormat="1" ht="22">
       <c r="A3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
@@ -1297,19 +1297,19 @@
         <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
@@ -1329,7 +1329,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>72</v>
@@ -1361,7 +1361,7 @@
         <v>76</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="4" t="s">
@@ -1371,7 +1371,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>72</v>
@@ -1403,7 +1403,7 @@
         <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="4" t="s">
@@ -1413,7 +1413,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>72</v>
@@ -1445,7 +1445,7 @@
         <v>78</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="4" t="s">
@@ -1455,7 +1455,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -1481,14 +1481,14 @@
         <v>79</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="10"/>
@@ -1498,7 +1498,7 @@
         <v>19</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4" t="s">
@@ -1519,17 +1519,17 @@
         <v>80</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>72</v>
@@ -1557,17 +1557,17 @@
         <v>81</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>72</v>
@@ -1595,7 +1595,7 @@
         <v>82</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="4" t="s">
@@ -1616,7 +1616,7 @@
         <v>45</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -1635,7 +1635,7 @@
         <v>83</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="4" t="s">
@@ -1656,7 +1656,7 @@
         <v>45</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -1675,7 +1675,7 @@
         <v>84</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="4" t="s">
@@ -1685,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>72</v>
@@ -1717,17 +1717,17 @@
         <v>85</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>72</v>
@@ -1739,7 +1739,7 @@
         <v>72</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -1759,17 +1759,17 @@
         <v>86</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>72</v>
@@ -1781,7 +1781,7 @@
         <v>72</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
@@ -1801,7 +1801,7 @@
         <v>87</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="4" t="s">
@@ -1811,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>72</v>
@@ -1843,7 +1843,7 @@
         <v>88</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="4" t="s">
@@ -1853,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>72</v>
@@ -1885,11 +1885,11 @@
         <v>89</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>22</v>
@@ -1929,7 +1929,7 @@
         <v>90</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="4" t="s">
@@ -1965,17 +1965,17 @@
         <v>91</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>72</v>
@@ -2005,17 +2005,17 @@
         <v>92</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>72</v>
@@ -2045,17 +2045,17 @@
         <v>93</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>72</v>
@@ -2085,17 +2085,17 @@
         <v>94</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>155</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>72</v>
@@ -2121,17 +2121,17 @@
         <v>95</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>72</v>
@@ -2159,7 +2159,7 @@
         <v>96</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="4" t="s">
@@ -2169,7 +2169,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>72</v>
@@ -2201,7 +2201,7 @@
         <v>97</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="4" t="s">
@@ -2211,7 +2211,7 @@
         <v>55</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>72</v>
@@ -2239,7 +2239,7 @@
         <v>98</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="4" t="s">
@@ -2249,7 +2249,7 @@
         <v>55</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>72</v>
@@ -2277,17 +2277,17 @@
         <v>99</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E28" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>155</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>72</v>
@@ -2313,17 +2313,17 @@
         <v>100</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>72</v>
@@ -2349,17 +2349,17 @@
         <v>101</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>72</v>

</xml_diff>